<commit_message>
Final Version Of database
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/Root/Resource.xlsx
+++ b/Luban/Config/Datas/Root/Resource.xlsx
@@ -5,27 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game\RootsPinkShark\Luban\Config\Datas\Root\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\刘文韬\Desktop\Datas\Root\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304F958E-69A5-4F61-B678-47761049358B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F3B73B-5D0B-413E-9368-C83566C2437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="1320" windowWidth="21600" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="159">
   <si>
     <t>##</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -354,6 +363,10 @@
     <t>地图promax8</t>
   </si>
   <si>
+    <t>USEHEART,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>TATTRI,9,1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -468,10 +481,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OPENEVENT,0,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ATTRIMINNEED,1,3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -528,15 +537,83 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TATTRI,0,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>OPENEVENT,119,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,120,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,121,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,122,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,123,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,124,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,125,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,126,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,127,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,128,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,129,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,130,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,131,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,132,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,133,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,134,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,135,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,136,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,137,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,138,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,139,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,140,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,141,0</t>
+  </si>
+  <si>
+    <t>OPENEVENT,142,0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,16 +628,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,18 +639,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,15 +655,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -889,18 +940,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="14.125" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -938,7 +990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -976,7 +1028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1066,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -1034,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -1054,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -1071,13 +1123,13 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -1094,13 +1146,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1117,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -1126,7 +1178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1143,7 +1195,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -1152,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1169,7 +1221,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -1178,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1195,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -1204,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1221,7 +1273,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -1230,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1247,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1256,7 +1308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
@@ -1273,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -1282,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
@@ -1299,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -1308,7 +1360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
@@ -1325,7 +1377,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -1334,7 +1386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1351,13 +1403,13 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
@@ -1374,13 +1426,13 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
       </c>
@@ -1397,13 +1449,13 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17</v>
       </c>
@@ -1420,7 +1472,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -1429,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
       </c>
@@ -1446,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -1455,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>19</v>
       </c>
@@ -1472,13 +1524,13 @@
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>20</v>
       </c>
@@ -1495,13 +1547,13 @@
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>21</v>
       </c>
@@ -1518,13 +1570,13 @@
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>22</v>
       </c>
@@ -1541,13 +1593,13 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>23</v>
       </c>
@@ -1564,13 +1616,13 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>24</v>
       </c>
@@ -1587,13 +1639,13 @@
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>25</v>
       </c>
@@ -1610,13 +1662,13 @@
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>26</v>
       </c>
@@ -1633,13 +1685,13 @@
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>27</v>
       </c>
@@ -1656,13 +1708,13 @@
         <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>28</v>
       </c>
@@ -1679,13 +1731,13 @@
         <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>29</v>
       </c>
@@ -1702,13 +1754,13 @@
         <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>30</v>
       </c>
@@ -1725,13 +1777,13 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>31</v>
       </c>
@@ -1748,13 +1800,13 @@
         <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>32</v>
       </c>
@@ -1771,13 +1823,13 @@
         <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>33</v>
       </c>
@@ -1794,13 +1846,13 @@
         <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>34</v>
       </c>
@@ -1817,13 +1869,13 @@
         <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>35</v>
       </c>
@@ -1840,13 +1892,13 @@
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>36</v>
       </c>
@@ -1863,13 +1915,13 @@
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>37</v>
       </c>
@@ -1886,13 +1938,13 @@
         <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>38</v>
       </c>
@@ -1909,13 +1961,13 @@
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>39</v>
       </c>
@@ -1935,13 +1987,13 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="K42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>40</v>
       </c>
@@ -1961,13 +2013,13 @@
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>41</v>
       </c>
@@ -1987,13 +2039,13 @@
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>42</v>
       </c>
@@ -2013,13 +2065,13 @@
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>43</v>
       </c>
@@ -2038,8 +2090,8 @@
       <c r="H46" t="b">
         <v>1</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>120</v>
+      <c r="I46" t="s">
+        <v>135</v>
       </c>
       <c r="J46" t="s">
         <v>121</v>
@@ -2048,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>44</v>
       </c>
@@ -2067,8 +2119,8 @@
       <c r="H47" t="b">
         <v>1</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>120</v>
+      <c r="I47" t="s">
+        <v>136</v>
       </c>
       <c r="J47" t="s">
         <v>121</v>
@@ -2077,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>45</v>
       </c>
@@ -2096,8 +2148,8 @@
       <c r="H48" t="b">
         <v>1</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>120</v>
+      <c r="I48" t="s">
+        <v>137</v>
       </c>
       <c r="J48" t="s">
         <v>122</v>
@@ -2106,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>46</v>
       </c>
@@ -2125,8 +2177,8 @@
       <c r="H49" t="b">
         <v>1</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>120</v>
+      <c r="I49" t="s">
+        <v>138</v>
       </c>
       <c r="J49" t="s">
         <v>122</v>
@@ -2135,7 +2187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>47</v>
       </c>
@@ -2154,8 +2206,8 @@
       <c r="H50" t="b">
         <v>1</v>
       </c>
-      <c r="I50" s="2" t="s">
-        <v>120</v>
+      <c r="I50" t="s">
+        <v>139</v>
       </c>
       <c r="J50" t="s">
         <v>122</v>
@@ -2164,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>48</v>
       </c>
@@ -2183,8 +2235,8 @@
       <c r="H51" t="b">
         <v>1</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>120</v>
+      <c r="I51" t="s">
+        <v>140</v>
       </c>
       <c r="J51" t="s">
         <v>123</v>
@@ -2193,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>49</v>
       </c>
@@ -2212,8 +2264,8 @@
       <c r="H52" t="b">
         <v>1</v>
       </c>
-      <c r="I52" s="2" t="s">
-        <v>120</v>
+      <c r="I52" t="s">
+        <v>141</v>
       </c>
       <c r="J52" t="s">
         <v>123</v>
@@ -2222,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>50</v>
       </c>
@@ -2241,8 +2293,8 @@
       <c r="H53" t="b">
         <v>1</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>120</v>
+      <c r="I53" t="s">
+        <v>142</v>
       </c>
       <c r="J53" t="s">
         <v>123</v>
@@ -2251,7 +2303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>51</v>
       </c>
@@ -2270,8 +2322,8 @@
       <c r="H54" t="b">
         <v>1</v>
       </c>
-      <c r="I54" s="2" t="s">
-        <v>120</v>
+      <c r="I54" t="s">
+        <v>143</v>
       </c>
       <c r="J54" t="s">
         <v>124</v>
@@ -2280,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>52</v>
       </c>
@@ -2299,8 +2351,8 @@
       <c r="H55" t="b">
         <v>1</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>120</v>
+      <c r="I55" t="s">
+        <v>144</v>
       </c>
       <c r="J55" t="s">
         <v>124</v>
@@ -2309,7 +2361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>53</v>
       </c>
@@ -2328,8 +2380,8 @@
       <c r="H56" t="b">
         <v>1</v>
       </c>
-      <c r="I56" s="2" t="s">
-        <v>120</v>
+      <c r="I56" t="s">
+        <v>145</v>
       </c>
       <c r="J56" t="s">
         <v>125</v>
@@ -2338,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>54</v>
       </c>
@@ -2357,8 +2409,8 @@
       <c r="H57" t="b">
         <v>1</v>
       </c>
-      <c r="I57" s="2" t="s">
-        <v>120</v>
+      <c r="I57" t="s">
+        <v>146</v>
       </c>
       <c r="J57" t="s">
         <v>125</v>
@@ -2367,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>55</v>
       </c>
@@ -2386,8 +2438,8 @@
       <c r="H58" t="b">
         <v>1</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>120</v>
+      <c r="I58" t="s">
+        <v>147</v>
       </c>
       <c r="J58" t="s">
         <v>126</v>
@@ -2396,7 +2448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>56</v>
       </c>
@@ -2415,8 +2467,8 @@
       <c r="H59" t="b">
         <v>1</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>120</v>
+      <c r="I59" t="s">
+        <v>148</v>
       </c>
       <c r="J59" t="s">
         <v>126</v>
@@ -2425,7 +2477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>57</v>
       </c>
@@ -2444,8 +2496,8 @@
       <c r="H60" t="b">
         <v>1</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>120</v>
+      <c r="I60" t="s">
+        <v>149</v>
       </c>
       <c r="J60" t="s">
         <v>125</v>
@@ -2454,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>58</v>
       </c>
@@ -2473,8 +2525,8 @@
       <c r="H61" t="b">
         <v>1</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>120</v>
+      <c r="I61" t="s">
+        <v>150</v>
       </c>
       <c r="J61" t="s">
         <v>125</v>
@@ -2483,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>59</v>
       </c>
@@ -2502,8 +2554,8 @@
       <c r="H62" t="b">
         <v>1</v>
       </c>
-      <c r="I62" s="3" t="s">
-        <v>120</v>
+      <c r="I62" t="s">
+        <v>151</v>
       </c>
       <c r="J62" t="s">
         <v>127</v>
@@ -2512,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>60</v>
       </c>
@@ -2531,8 +2583,8 @@
       <c r="H63" t="b">
         <v>1</v>
       </c>
-      <c r="I63" s="3" t="s">
-        <v>120</v>
+      <c r="I63" t="s">
+        <v>152</v>
       </c>
       <c r="J63" t="s">
         <v>128</v>
@@ -2541,7 +2593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>61</v>
       </c>
@@ -2560,8 +2612,8 @@
       <c r="H64" t="b">
         <v>1</v>
       </c>
-      <c r="I64" s="3" t="s">
-        <v>120</v>
+      <c r="I64" t="s">
+        <v>153</v>
       </c>
       <c r="J64" t="s">
         <v>129</v>
@@ -2570,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>62</v>
       </c>
@@ -2589,8 +2641,8 @@
       <c r="H65" t="b">
         <v>1</v>
       </c>
-      <c r="I65" s="3" t="s">
-        <v>120</v>
+      <c r="I65" t="s">
+        <v>154</v>
       </c>
       <c r="J65" t="s">
         <v>130</v>
@@ -2599,7 +2651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>63</v>
       </c>
@@ -2618,8 +2670,8 @@
       <c r="H66" t="b">
         <v>1</v>
       </c>
-      <c r="I66" s="3" t="s">
-        <v>120</v>
+      <c r="I66" t="s">
+        <v>155</v>
       </c>
       <c r="J66" t="s">
         <v>131</v>
@@ -2628,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>64</v>
       </c>
@@ -2647,8 +2699,8 @@
       <c r="H67" t="b">
         <v>1</v>
       </c>
-      <c r="I67" s="3" t="s">
-        <v>120</v>
+      <c r="I67" t="s">
+        <v>156</v>
       </c>
       <c r="J67" t="s">
         <v>132</v>
@@ -2657,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>65</v>
       </c>
@@ -2676,8 +2728,8 @@
       <c r="H68" t="b">
         <v>1</v>
       </c>
-      <c r="I68" s="3" t="s">
-        <v>120</v>
+      <c r="I68" t="s">
+        <v>157</v>
       </c>
       <c r="J68" t="s">
         <v>133</v>
@@ -2686,7 +2738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>66</v>
       </c>
@@ -2705,8 +2757,8 @@
       <c r="H69" t="b">
         <v>1</v>
       </c>
-      <c r="I69" s="3" t="s">
-        <v>120</v>
+      <c r="I69" t="s">
+        <v>158</v>
       </c>
       <c r="J69" t="s">
         <v>134</v>

</xml_diff>